<commit_message>
add new school mockup data
</commit_message>
<xml_diff>
--- a/perforkid/database/form_car.xlsx
+++ b/perforkid/database/form_car.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS_code_Project\project_childcare_mobileapp\perforkid\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CEE42E3-A9D5-43E4-9749-D5C41AF8FD14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D786F60-F079-463D-90C1-F192B32C7463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4575" yWindow="1815" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,30 +27,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
-    <t>รหัสประจำตัว</t>
-  </si>
-  <si>
     <t>099-999-9999</t>
   </si>
   <si>
-    <t>ลำดับ</t>
-  </si>
-  <si>
-    <t>ชื่อ-สกุล</t>
-  </si>
-  <si>
-    <t>เบอร์รถ</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
-    <t>เบอร์โทร (บิดา)</t>
-  </si>
-  <si>
-    <t>เบอร์โทร (มารดา)</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -63,19 +45,37 @@
     <t>ด.ช. โชคชัย ใจดี</t>
   </si>
   <si>
-    <t>ที่อยู่ที่ไปรับ-ส่ง</t>
-  </si>
-  <si>
     <t>12/34 กรุงเทพ ประเทศไทย 10000</t>
   </si>
   <si>
     <t>24/62 กรุงเทพ ประเทศไทย 10000</t>
   </si>
   <si>
-    <t>ห้องเรียน</t>
-  </si>
-  <si>
     <t>1/1</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>name-surname</t>
+  </si>
+  <si>
+    <t>class-room</t>
+  </si>
+  <si>
+    <t>car-number</t>
+  </si>
+  <si>
+    <t>father-phone</t>
+  </si>
+  <si>
+    <t>mother-phone</t>
+  </si>
+  <si>
+    <t>address</t>
   </si>
 </sst>
 </file>
@@ -630,7 +630,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -646,28 +646,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="25.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="H1" s="14" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -678,48 +678,48 @@
         <v>123456</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>16</v>
-      </c>
       <c r="E3" s="20" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>